<commit_message>
eta.fu --> etafu, phi.u --> phiu
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Efficiency-sample-2018.xlsx
+++ b/inst/extdata/GH-ZA-Efficiency-sample-2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8307070-F7DD-9B44-BA60-091A430A0668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF029BA-1D30-9F49-BC10-A3080B5F51A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28540" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,15 +67,9 @@
     <t>MD</t>
   </si>
   <si>
-    <t>eta.fu</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>phi.u</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -215,6 +209,12 @@
   </si>
   <si>
     <t>Edot_machine_max [%]</t>
+  </si>
+  <si>
+    <t>phiu</t>
+  </si>
+  <si>
+    <t>etafu</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:K135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -621,10 +621,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -662,7 +662,7 @@
         <v>0.115406110283159</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J2" s="3">
         <v>0.3</v>
@@ -697,13 +697,13 @@
         <v>0.115406110283159</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>14</v>
@@ -732,7 +732,7 @@
         <v>3.4929210134128197E-2</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J4" s="3">
         <v>0.3</v>
@@ -758,7 +758,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -767,13 +767,13 @@
         <v>3.4929210134128197E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>14</v>
@@ -802,7 +802,7 @@
         <v>3.4929210134128197E-2</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J6" s="3">
         <v>0.3</v>
@@ -828,7 +828,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -837,13 +837,13 @@
         <v>3.4929210134128197E-2</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -863,7 +863,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>14</v>
@@ -872,7 +872,7 @@
         <v>3.4836065573770503E-2</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J8" s="3">
         <v>0.85</v>
@@ -898,7 +898,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -907,13 +907,13 @@
         <v>3.4836065573770503E-2</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -933,7 +933,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>14</v>
@@ -942,7 +942,7 @@
         <v>1.31333830104322E-2</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J10" s="3">
         <v>0.3</v>
@@ -968,7 +968,7 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -977,13 +977,13 @@
         <v>1.31333830104322E-2</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1003,7 +1003,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>14</v>
@@ -1012,7 +1012,7 @@
         <v>1.1736214605067101E-2</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J12" s="3">
         <v>0.3</v>
@@ -1038,7 +1038,7 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
@@ -1047,13 +1047,13 @@
         <v>1.1736214605067101E-2</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1073,7 +1073,7 @@
         <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>14</v>
@@ -1082,7 +1082,7 @@
         <v>5.7982218786238899E-3</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J14" s="3">
         <v>0.3</v>
@@ -1108,7 +1108,7 @@
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1117,13 +1117,13 @@
         <v>5.7982218786238899E-3</v>
       </c>
       <c r="I15" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1143,7 +1143,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>14</v>
@@ -1152,7 +1152,7 @@
         <v>3.5488077496274202E-3</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J16" s="3">
         <v>0.1</v>
@@ -1178,7 +1178,7 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
@@ -1187,13 +1187,13 @@
         <v>3.5488077496274202E-3</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1213,22 +1213,22 @@
         <v>12</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H18" s="3">
         <v>2.9592026825633399E-2</v>
       </c>
       <c r="I18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="K18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1248,16 +1248,16 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H19" s="2">
         <v>2.9592026825633399E-2</v>
       </c>
       <c r="I19" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1279,16 +1279,16 @@
         <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H20" s="3">
         <v>6.24275222265172E-2</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J20" s="3">
         <v>0.85</v>
@@ -1314,22 +1314,22 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H21" s="2">
         <v>6.24275222265172E-2</v>
       </c>
       <c r="I21" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1349,16 +1349,16 @@
         <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H22" s="3">
         <v>7.73096250483185E-3</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J22" s="3">
         <v>0.85</v>
@@ -1384,22 +1384,22 @@
         <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H23" s="2">
         <v>7.73096250483185E-3</v>
       </c>
       <c r="I23" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1419,16 +1419,16 @@
         <v>12</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H24" s="3">
         <v>0.12760804769001499</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J24" s="3">
         <v>0.85</v>
@@ -1454,22 +1454,22 @@
         <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H25" s="2">
         <v>0.12760804769001499</v>
       </c>
       <c r="I25" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1489,16 +1489,16 @@
         <v>12</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H26" s="3">
         <v>5.2570545032856603E-2</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J26" s="3">
         <v>0.85</v>
@@ -1524,22 +1524,22 @@
         <v>12</v>
       </c>
       <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
         <v>31</v>
-      </c>
-      <c r="G27" t="s">
-        <v>33</v>
       </c>
       <c r="H27" s="2">
         <v>5.2570545032856603E-2</v>
       </c>
       <c r="I27" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1559,16 +1559,16 @@
         <v>12</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H28" s="3">
         <v>2.75707898658718E-2</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J28" s="3">
         <v>0.97</v>
@@ -1594,22 +1594,22 @@
         <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H29" s="2">
         <v>2.75707898658718E-2</v>
       </c>
       <c r="I29" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1629,16 +1629,16 @@
         <v>12</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H30" s="3">
         <v>3.5488077496274202E-3</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J30" s="3">
         <v>0.85</v>
@@ -1664,22 +1664,22 @@
         <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H31" s="2">
         <v>3.5488077496274202E-3</v>
       </c>
       <c r="I31" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1699,16 +1699,16 @@
         <v>12</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H32" s="3">
         <v>9.3144560357675101E-4</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J32" s="3">
         <v>0.45</v>
@@ -1734,22 +1734,22 @@
         <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H33" s="2">
         <v>9.3144560357675101E-4</v>
       </c>
       <c r="I33" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1769,16 +1769,16 @@
         <v>12</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H34" s="3">
         <v>3.8654812524159299E-4</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J34" s="3">
         <v>0.65</v>
@@ -1804,22 +1804,22 @@
         <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H35" s="2">
         <v>3.8654812524159299E-4</v>
       </c>
       <c r="I35" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1839,16 +1839,16 @@
         <v>12</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H36" s="3">
         <v>0.565906455353692</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J36" s="3">
         <v>0.12</v>
@@ -1874,22 +1874,22 @@
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H37" s="2">
         <v>0.565906455353692</v>
       </c>
       <c r="I37" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1909,16 +1909,16 @@
         <v>12</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H38" s="3">
         <v>9.6125186289120701E-2</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J38" s="3">
         <v>0.14000000000000001</v>
@@ -1944,22 +1944,22 @@
         <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H39" s="2">
         <v>9.6125186289120701E-2</v>
       </c>
       <c r="I39" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1979,16 +1979,16 @@
         <v>12</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H40" s="3">
         <v>3.2470042520293799E-2</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J40" s="3">
         <v>0.16</v>
@@ -2014,22 +2014,22 @@
         <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G41" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H41" s="2">
         <v>3.2470042520293799E-2</v>
       </c>
       <c r="I41" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2049,16 +2049,16 @@
         <v>12</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="H42" s="3">
         <v>6.7064083457526102E-3</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J42" s="3">
         <v>0.18</v>
@@ -2084,22 +2084,22 @@
         <v>12</v>
       </c>
       <c r="F43" t="s">
+        <v>34</v>
+      </c>
+      <c r="G43" t="s">
         <v>36</v>
-      </c>
-      <c r="G43" t="s">
-        <v>38</v>
       </c>
       <c r="H43" s="2">
         <v>6.7064083457526102E-3</v>
       </c>
       <c r="I43" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2119,16 +2119,16 @@
         <v>12</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H44" s="3">
         <v>3.5488077496274202E-3</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J44" s="3">
         <v>0.7</v>
@@ -2154,27 +2154,27 @@
         <v>12</v>
       </c>
       <c r="F45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H45" s="2">
         <v>3.5488077496274202E-3</v>
       </c>
       <c r="I45" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>9</v>
@@ -2189,7 +2189,7 @@
         <v>12</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>14</v>
@@ -2198,7 +2198,7 @@
         <v>9.9232274574740306E-2</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J46" s="3">
         <v>0.6</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
@@ -2224,7 +2224,7 @@
         <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G47" t="s">
         <v>14</v>
@@ -2233,18 +2233,18 @@
         <v>9.9232274574740306E-2</v>
       </c>
       <c r="I47" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>9</v>
@@ -2259,7 +2259,7 @@
         <v>12</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>14</v>
@@ -2268,7 +2268,7 @@
         <v>9.6400985111384702E-2</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J48" s="3">
         <v>0.87</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -2294,7 +2294,7 @@
         <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G49" t="s">
         <v>14</v>
@@ -2303,18 +2303,18 @@
         <v>9.6400985111384702E-2</v>
       </c>
       <c r="I49" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>9</v>
@@ -2329,7 +2329,7 @@
         <v>12</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>14</v>
@@ -2338,7 +2338,7 @@
         <v>7.6681965744990505E-2</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J50" s="3">
         <v>0.3</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -2364,7 +2364,7 @@
         <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G51" t="s">
         <v>14</v>
@@ -2373,18 +2373,18 @@
         <v>7.6681965744990505E-2</v>
       </c>
       <c r="I51" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>9</v>
@@ -2408,7 +2408,7 @@
         <v>7.5189372737788696E-2</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J52" s="3">
         <v>0.3</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
@@ -2443,33 +2443,33 @@
         <v>7.5189372737788696E-2</v>
       </c>
       <c r="I53" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>14</v>
@@ -2478,7 +2478,7 @@
         <v>4.6587559237284998E-2</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J54" s="3">
         <v>0.3</v>
@@ -2489,22 +2489,22 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" t="s">
         <v>42</v>
-      </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" t="s">
-        <v>44</v>
       </c>
       <c r="G55" t="s">
         <v>14</v>
@@ -2513,18 +2513,18 @@
         <v>4.6587559237284998E-2</v>
       </c>
       <c r="I55" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>9</v>
@@ -2539,7 +2539,7 @@
         <v>12</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>14</v>
@@ -2548,7 +2548,7 @@
         <v>3.12325086756969E-2</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J56" s="3">
         <v>0.3</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -2574,7 +2574,7 @@
         <v>12</v>
       </c>
       <c r="F57" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G57" t="s">
         <v>14</v>
@@ -2583,18 +2583,18 @@
         <v>3.12325086756969E-2</v>
       </c>
       <c r="I57" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>9</v>
@@ -2609,7 +2609,7 @@
         <v>12</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>14</v>
@@ -2618,7 +2618,7 @@
         <v>3.1213851263106801E-2</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J58" s="3">
         <v>0.3</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
@@ -2644,7 +2644,7 @@
         <v>12</v>
       </c>
       <c r="F59" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G59" t="s">
         <v>14</v>
@@ -2653,18 +2653,18 @@
         <v>3.1213851263106801E-2</v>
       </c>
       <c r="I59" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>9</v>
@@ -2679,7 +2679,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>14</v>
@@ -2688,7 +2688,7 @@
         <v>1.38027538340983E-2</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J60" s="3">
         <v>0.12</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
@@ -2714,7 +2714,7 @@
         <v>12</v>
       </c>
       <c r="F61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G61" t="s">
         <v>14</v>
@@ -2723,18 +2723,18 @@
         <v>1.38027538340983E-2</v>
       </c>
       <c r="I61" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>9</v>
@@ -2749,7 +2749,7 @@
         <v>12</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>14</v>
@@ -2758,7 +2758,7 @@
         <v>1.14556513302735E-2</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J62" s="3">
         <v>0.3</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
@@ -2784,7 +2784,7 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G63" t="s">
         <v>14</v>
@@ -2793,18 +2793,18 @@
         <v>1.14556513302735E-2</v>
       </c>
       <c r="I63" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>9</v>
@@ -2819,7 +2819,7 @@
         <v>12</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>14</v>
@@ -2828,7 +2828,7 @@
         <v>9.6831971342214301E-3</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J64" s="3">
         <v>0.3</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
@@ -2854,7 +2854,7 @@
         <v>12</v>
       </c>
       <c r="F65" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G65" t="s">
         <v>14</v>
@@ -2863,18 +2863,18 @@
         <v>9.6831971342214301E-3</v>
       </c>
       <c r="I65" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>9</v>
@@ -2889,7 +2889,7 @@
         <v>12</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>14</v>
@@ -2898,7 +2898,7 @@
         <v>3.0225008395835702E-3</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J66" s="3">
         <v>0.45</v>
@@ -2909,7 +2909,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
@@ -2924,7 +2924,7 @@
         <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G67" t="s">
         <v>14</v>
@@ -2933,18 +2933,18 @@
         <v>3.0225008395835702E-3</v>
       </c>
       <c r="I67" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>9</v>
@@ -2959,7 +2959,7 @@
         <v>12</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>14</v>
@@ -2968,7 +2968,7 @@
         <v>1.92171349677227E-3</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J68" s="3">
         <v>0.3</v>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
@@ -2994,7 +2994,7 @@
         <v>12</v>
       </c>
       <c r="F69" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G69" t="s">
         <v>14</v>
@@ -3003,18 +3003,18 @@
         <v>1.92171349677227E-3</v>
       </c>
       <c r="I69" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>9</v>
@@ -3029,7 +3029,7 @@
         <v>12</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>14</v>
@@ -3038,7 +3038,7 @@
         <v>6.3435202806074896E-4</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J70" s="3">
         <v>0.3</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -3064,7 +3064,7 @@
         <v>12</v>
       </c>
       <c r="F71" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G71" t="s">
         <v>14</v>
@@ -3073,18 +3073,18 @@
         <v>6.3435202806074896E-4</v>
       </c>
       <c r="I71" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>9</v>
@@ -3099,27 +3099,27 @@
         <v>12</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H72" s="3">
         <v>0.116858838016344</v>
       </c>
       <c r="I72" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J72" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J72" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="K72" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
@@ -3134,23 +3134,23 @@
         <v>12</v>
       </c>
       <c r="F73" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G73" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H73" s="2">
         <v>0.116858838016344</v>
       </c>
       <c r="I73" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>9</v>
@@ -3165,27 +3165,27 @@
         <v>12</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H74" s="3">
         <v>2.77995447591328E-3</v>
       </c>
       <c r="I74" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J74" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J74" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="K74" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
@@ -3200,23 +3200,23 @@
         <v>12</v>
       </c>
       <c r="F75" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G75" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H75" s="2">
         <v>2.77995447591328E-3</v>
       </c>
       <c r="I75" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>9</v>
@@ -3231,27 +3231,27 @@
         <v>12</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H76" s="3">
         <v>2.1549311541475399E-3</v>
       </c>
       <c r="I76" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J76" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J76" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="K76" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
@@ -3266,23 +3266,23 @@
         <v>12</v>
       </c>
       <c r="F77" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G77" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H77" s="2">
         <v>2.1549311541475399E-3</v>
       </c>
       <c r="I77" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>9</v>
@@ -3297,16 +3297,16 @@
         <v>12</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H78" s="3">
         <v>0.21550504290230299</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J78" s="3">
         <v>0.85</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
@@ -3332,27 +3332,27 @@
         <v>12</v>
       </c>
       <c r="F79" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G79" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H79" s="2">
         <v>0.21550504290230299</v>
       </c>
       <c r="I79" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>9</v>
@@ -3367,16 +3367,16 @@
         <v>12</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H80" s="3">
         <v>3.1419082801597102E-2</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J80" s="3">
         <v>0.9</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
@@ -3402,27 +3402,27 @@
         <v>12</v>
       </c>
       <c r="F81" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G81" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H81" s="2">
         <v>3.1419082801597102E-2</v>
       </c>
       <c r="I81" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>9</v>
@@ -3437,16 +3437,16 @@
         <v>12</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H82" s="3">
         <v>1.9627598044703199E-2</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J82" s="3">
         <v>0.8</v>
@@ -3457,7 +3457,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -3472,27 +3472,27 @@
         <v>12</v>
       </c>
       <c r="F83" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G83" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H83" s="2">
         <v>1.9627598044703199E-2</v>
       </c>
       <c r="I83" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>9</v>
@@ -3507,16 +3507,16 @@
         <v>12</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H84" s="3">
         <v>1.7461990064729802E-2</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J84" s="3">
         <v>0.8</v>
@@ -3527,7 +3527,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -3542,27 +3542,27 @@
         <v>12</v>
       </c>
       <c r="F85" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G85" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H85" s="2">
         <v>1.7461990064729802E-2</v>
       </c>
       <c r="I85" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>9</v>
@@ -3577,16 +3577,16 @@
         <v>12</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H86" s="3">
         <v>3.17176014030374E-3</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J86" s="3">
         <v>0.8</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
@@ -3612,27 +3612,27 @@
         <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G87" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H87" s="2">
         <v>3.17176014030374E-3</v>
       </c>
       <c r="I87" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K87" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>9</v>
@@ -3647,16 +3647,16 @@
         <v>12</v>
       </c>
       <c r="F88" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G88" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H88" s="3">
         <v>6.4517332736296104E-2</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J88" s="3">
         <v>0.8</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -3682,27 +3682,27 @@
         <v>12</v>
       </c>
       <c r="F89" t="s">
+        <v>29</v>
+      </c>
+      <c r="G89" t="s">
         <v>31</v>
-      </c>
-      <c r="G89" t="s">
-        <v>33</v>
       </c>
       <c r="H89" s="2">
         <v>6.4517332736296104E-2</v>
       </c>
       <c r="I89" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K89" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>9</v>
@@ -3717,16 +3717,16 @@
         <v>12</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H90" s="3">
         <v>2.8265980073883399E-2</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J90" s="3">
         <v>0.2</v>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
@@ -3752,27 +3752,27 @@
         <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G91" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H91" s="2">
         <v>2.8265980073883399E-2</v>
       </c>
       <c r="I91" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K91" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>9</v>
@@ -3787,16 +3787,16 @@
         <v>12</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H92" s="3">
         <v>2.3004589723497101E-2</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J92" s="3">
         <v>0.3</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
@@ -3822,27 +3822,27 @@
         <v>12</v>
       </c>
       <c r="F93" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G93" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H93" s="2">
         <v>2.3004589723497101E-2</v>
       </c>
       <c r="I93" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K93" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>9</v>
@@ -3857,16 +3857,16 @@
         <v>12</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H94" s="3">
         <v>1.68598524762908E-2</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J94" s="3">
         <v>0.14000000000000001</v>
@@ -3877,7 +3877,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
@@ -3892,27 +3892,27 @@
         <v>12</v>
       </c>
       <c r="F95" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G95" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H95" s="2">
         <v>1.68598524762908E-2</v>
       </c>
       <c r="I95" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K95" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>9</v>
@@ -3927,16 +3927,16 @@
         <v>12</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H96" s="3">
         <v>1.5776004817100699E-2</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J96" s="3">
         <v>0.4</v>
@@ -3947,7 +3947,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
@@ -3962,27 +3962,27 @@
         <v>12</v>
       </c>
       <c r="F97" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G97" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H97" s="2">
         <v>1.5776004817100699E-2</v>
       </c>
       <c r="I97" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K97" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>9</v>
@@ -3997,16 +3997,16 @@
         <v>12</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H98" s="3">
         <v>1.0709354826672599E-2</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J98" s="3">
         <v>0.4</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
@@ -4032,27 +4032,27 @@
         <v>12</v>
       </c>
       <c r="F99" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G99" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H99" s="2">
         <v>1.0709354826672599E-2</v>
       </c>
       <c r="I99" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K99" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>9</v>
@@ -4067,16 +4067,16 @@
         <v>12</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H100" s="3">
         <v>8.9163774767715195E-3</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J100" s="3">
         <v>0.4</v>
@@ -4087,7 +4087,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
@@ -4102,27 +4102,27 @@
         <v>12</v>
       </c>
       <c r="F101" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G101" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H101" s="2">
         <v>8.9163774767715195E-3</v>
       </c>
       <c r="I101" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>9</v>
@@ -4137,16 +4137,16 @@
         <v>12</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H102" s="3">
         <v>3.6128255306337501E-3</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J102" s="3">
         <v>0.3</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
@@ -4172,27 +4172,27 @@
         <v>12</v>
       </c>
       <c r="F103" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G103" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H103" s="2">
         <v>3.6128255306337501E-3</v>
       </c>
       <c r="I103" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K103" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>9</v>
@@ -4207,16 +4207,16 @@
         <v>12</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H104" s="3">
         <v>2.3182297154899899E-3</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J104" s="3">
         <v>0.25</v>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
@@ -4242,27 +4242,27 @@
         <v>12</v>
       </c>
       <c r="F105" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H105" s="2">
         <v>2.3182297154899899E-3</v>
       </c>
       <c r="I105" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K105" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>9</v>
@@ -4277,16 +4277,16 @@
         <v>12</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H106" s="3">
         <v>2.0523153849024201E-4</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J106" s="3">
         <v>0.85</v>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
@@ -4312,27 +4312,27 @@
         <v>12</v>
       </c>
       <c r="F107" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G107" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H107" s="2">
         <v>2.0523153849024201E-4</v>
       </c>
       <c r="I107" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J107" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K107" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>9</v>
@@ -4347,16 +4347,16 @@
         <v>12</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H108" s="3">
         <v>5.5972237770065998E-5</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J108" s="3">
         <v>0.85</v>
@@ -4367,7 +4367,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B109" t="s">
         <v>9</v>
@@ -4382,27 +4382,27 @@
         <v>12</v>
       </c>
       <c r="F109" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G109" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H109" s="2">
         <v>5.5972237770065998E-5</v>
       </c>
       <c r="I109" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J109" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K109" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>9</v>
@@ -4417,16 +4417,16 @@
         <v>12</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H110" s="3">
         <v>6.0935109519011897E-2</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J110" s="3">
         <v>0.12</v>
@@ -4437,7 +4437,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
@@ -4452,27 +4452,27 @@
         <v>12</v>
       </c>
       <c r="F111" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G111" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H111" s="2">
         <v>6.0935109519011897E-2</v>
       </c>
       <c r="I111" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J111" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K111" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>9</v>
@@ -4487,16 +4487,16 @@
         <v>12</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H112" s="3">
         <v>1.51311616105079E-2</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J112" s="3">
         <v>0.14000000000000001</v>
@@ -4507,7 +4507,7 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B113" t="s">
         <v>9</v>
@@ -4522,27 +4522,27 @@
         <v>12</v>
       </c>
       <c r="F113" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H113" s="2">
         <v>1.51311616105079E-2</v>
       </c>
       <c r="I113" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J113" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K113" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>9</v>
@@ -4557,16 +4557,16 @@
         <v>12</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H114" s="3">
         <v>2.7053248255531899E-3</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J114" s="3">
         <v>0.16</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B115" t="s">
         <v>9</v>
@@ -4592,27 +4592,27 @@
         <v>12</v>
       </c>
       <c r="F115" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G115" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H115" s="2">
         <v>2.7053248255531899E-3</v>
       </c>
       <c r="I115" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J115" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K115" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>9</v>
@@ -4627,16 +4627,16 @@
         <v>12</v>
       </c>
       <c r="F116" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G116" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="H116" s="3">
         <v>8.7689839173103496E-4</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J116" s="3">
         <v>0.16</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B117" t="s">
         <v>9</v>
@@ -4662,27 +4662,27 @@
         <v>12</v>
       </c>
       <c r="F117" t="s">
+        <v>34</v>
+      </c>
+      <c r="G117" t="s">
         <v>36</v>
-      </c>
-      <c r="G117" t="s">
-        <v>38</v>
       </c>
       <c r="H117" s="2">
         <v>8.7689839173103496E-4</v>
       </c>
       <c r="I117" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J117" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K117" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>9</v>
@@ -4697,16 +4697,16 @@
         <v>12</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H118" s="3">
         <v>8.2092615396096901E-4</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J118" s="3">
         <v>0.16</v>
@@ -4717,7 +4717,7 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B119" t="s">
         <v>9</v>
@@ -4732,27 +4732,27 @@
         <v>12</v>
       </c>
       <c r="F119" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G119" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H119" s="2">
         <v>8.2092615396096901E-4</v>
       </c>
       <c r="I119" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J119" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K119" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>9</v>
@@ -4767,16 +4767,16 @@
         <v>12</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H120" s="3">
         <v>5.5972237770065998E-5</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J120" s="3">
         <v>0.16</v>
@@ -4787,7 +4787,7 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B121" t="s">
         <v>9</v>
@@ -4802,27 +4802,27 @@
         <v>12</v>
       </c>
       <c r="F121" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G121" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H121" s="2">
         <v>5.5972237770065998E-5</v>
       </c>
       <c r="I121" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J121" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K121" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>9</v>
@@ -4837,16 +4837,16 @@
         <v>12</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H122" s="3">
         <v>9.3287062950110104E-6</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J122" s="3">
         <v>0.85</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B123" t="s">
         <v>9</v>
@@ -4872,27 +4872,27 @@
         <v>12</v>
       </c>
       <c r="F123" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G123" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H123" s="2">
         <v>9.3287062950110104E-6</v>
       </c>
       <c r="I123" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J123" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K123" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>9</v>
@@ -4907,16 +4907,16 @@
         <v>12</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H124" s="3">
         <v>9.4535601384916498E-2</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J124" s="3">
         <v>0.16</v>
@@ -4927,7 +4927,7 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B125" t="s">
         <v>9</v>
@@ -4942,27 +4942,27 @@
         <v>12</v>
       </c>
       <c r="F125" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G125" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H125" s="2">
         <v>9.4535601384916498E-2</v>
       </c>
       <c r="I125" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J125" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K125" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>9</v>
@@ -4977,16 +4977,16 @@
         <v>12</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H126" s="3">
         <v>6.0935109519011897E-2</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J126" s="3">
         <v>0.85</v>
@@ -4997,7 +4997,7 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B127" t="s">
         <v>9</v>
@@ -5012,27 +5012,27 @@
         <v>12</v>
       </c>
       <c r="F127" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G127" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H127" s="2">
         <v>6.0935109519011897E-2</v>
       </c>
       <c r="I127" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J127" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K127" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>9</v>
@@ -5047,16 +5047,16 @@
         <v>12</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H128" s="3">
         <v>2.3362938431431599E-2</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J128" s="3">
         <v>0.85</v>
@@ -5067,7 +5067,7 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B129" t="s">
         <v>9</v>
@@ -5082,27 +5082,27 @@
         <v>12</v>
       </c>
       <c r="F129" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G129" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H129" s="2">
         <v>2.3362938431431599E-2</v>
       </c>
       <c r="I129" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J129" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K129" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>9</v>
@@ -5117,16 +5117,16 @@
         <v>12</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H130" s="3">
         <v>1.02988917496922E-2</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J130" s="3">
         <v>0.3</v>
@@ -5137,7 +5137,7 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B131" t="s">
         <v>9</v>
@@ -5152,27 +5152,27 @@
         <v>12</v>
       </c>
       <c r="F131" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G131" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H131" s="2">
         <v>1.02988917496922E-2</v>
       </c>
       <c r="I131" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J131" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K131" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>9</v>
@@ -5187,16 +5187,16 @@
         <v>12</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H132" s="3">
         <v>2.7053248255531899E-3</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J132" s="3">
         <v>0.32</v>
@@ -5207,7 +5207,7 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B133" t="s">
         <v>9</v>
@@ -5222,27 +5222,27 @@
         <v>12</v>
       </c>
       <c r="F133" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G133" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H133" s="2">
         <v>2.7053248255531899E-3</v>
       </c>
       <c r="I133" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J133" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K133" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>9</v>
@@ -5257,16 +5257,16 @@
         <v>12</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H134" s="3">
         <v>2.6120377626030799E-4</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J134" s="3">
         <v>0.85</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B135" t="s">
         <v>9</v>
@@ -5292,22 +5292,22 @@
         <v>12</v>
       </c>
       <c r="F135" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G135" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H135" s="2">
         <v>2.6120377626030799E-4</v>
       </c>
       <c r="I135" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J135" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K135" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>